<commit_message>
streamline projection for base om
</commit_message>
<xml_diff>
--- a/sf_fitted_sizes_y2plus.xlsx
+++ b/sf_fitted_sizes_y2plus.xlsx
@@ -428,7 +428,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>0.02286941666726232</v>
+        <v>0.05628289797049125</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -444,12 +444,12 @@
         </is>
       </c>
       <c r="E4">
-        <v>0.02286941666726232</v>
+        <v>0.05628289797049125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>0.02286941666726232</v>
+        <v>0.06452247115702553</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -465,12 +465,12 @@
         </is>
       </c>
       <c r="E5">
-        <v>0.04573883333452464</v>
+        <v>0.1208053691275168</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>0.04573883333452464</v>
+        <v>0.1500728335373864</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -486,12 +486,12 @@
         </is>
       </c>
       <c r="E6">
-        <v>0.09147766666904927</v>
+        <v>0.2708782026649032</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>0.09265705524542005</v>
+        <v>0.1671954172959544</v>
       </c>
       <c r="B7">
         <v>13</v>
@@ -507,12 +507,12 @@
         </is>
       </c>
       <c r="E7">
-        <v>0.1841347219144693</v>
+        <v>0.4380736199608576</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>0.0670857665668356</v>
+        <v>0.07843680461845057</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -528,12 +528,12 @@
         </is>
       </c>
       <c r="E8">
-        <v>0.2512204884813049</v>
+        <v>0.5165104245793082</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>0.06960179552975991</v>
+        <v>0.04398609460316893</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -549,12 +549,12 @@
         </is>
       </c>
       <c r="E9">
-        <v>0.3208222840110648</v>
+        <v>0.5604965191824771</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>0.240212861768511</v>
+        <v>0.2706279770149868</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -570,12 +570,12 @@
         </is>
       </c>
       <c r="E10">
-        <v>0.5610351457795759</v>
+        <v>0.8311244961974638</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>0.2489689284718698</v>
+        <v>0.04199322603419155</v>
       </c>
       <c r="B11">
         <v>17</v>
@@ -591,12 +591,12 @@
         </is>
       </c>
       <c r="E11">
-        <v>0.8100040742514456</v>
+        <v>0.8731177222316554</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>0.05330478974718197</v>
+        <v>0.0395177794260896</v>
       </c>
       <c r="B12">
         <v>18</v>
@@ -612,12 +612,12 @@
         </is>
       </c>
       <c r="E12">
-        <v>0.8633088639986276</v>
+        <v>0.912635501657745</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>0.02977420069619665</v>
+        <v>0.01891884645975388</v>
       </c>
       <c r="B13">
         <v>19</v>
@@ -633,12 +633,12 @@
         </is>
       </c>
       <c r="E13">
-        <v>0.8930830646948242</v>
+        <v>0.9315543481174988</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>0.05509531604039942</v>
+        <v>0.034414963493865</v>
       </c>
       <c r="B14">
         <v>20</v>
@@ -654,12 +654,12 @@
         </is>
       </c>
       <c r="E14">
-        <v>0.9481783807352238</v>
+        <v>0.9659693116113639</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>0.01957427646297792</v>
+        <v>0.01799837353327554</v>
       </c>
       <c r="B15">
         <v>21</v>
@@ -675,12 +675,12 @@
         </is>
       </c>
       <c r="E15">
-        <v>0.9677526571982016</v>
+        <v>0.9839676851446394</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>0.01665797016504292</v>
+        <v>0.008266383077596761</v>
       </c>
       <c r="B16">
         <v>22</v>
@@ -696,12 +696,12 @@
         </is>
       </c>
       <c r="E16">
-        <v>0.9844106273632446</v>
+        <v>0.9922340682222361</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>0.01275884005346562</v>
+        <v>0.006729282656681472</v>
       </c>
       <c r="B17">
         <v>23</v>
@@ -717,12 +717,12 @@
         </is>
       </c>
       <c r="E17">
-        <v>0.9971694674167102</v>
+        <v>0.9989633508789176</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>0.002555341915470004</v>
+        <v>0.0009472828175408181</v>
       </c>
       <c r="B18">
         <v>24</v>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="E18">
-        <v>0.9997248093321802</v>
+        <v>0.9999106336964585</v>
       </c>
     </row>
     <row r="19">
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="E19">
-        <v>0.9997248093321802</v>
+        <v>0.9999106336964585</v>
       </c>
     </row>
     <row r="20">
@@ -780,12 +780,12 @@
         </is>
       </c>
       <c r="E20">
-        <v>0.9997248093321802</v>
+        <v>0.9999106336964585</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>0.0002751906678198466</v>
+        <v>8.936630354158661e-05</v>
       </c>
       <c r="B21">
         <v>27</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>0.002279929703798317</v>
+        <v>0.003019541594534142</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -927,12 +927,12 @@
         </is>
       </c>
       <c r="E27">
-        <v>0.002279929703798317</v>
+        <v>0.003019541594534142</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>0.006839136770993293</v>
+        <v>0.005622414343171251</v>
       </c>
       <c r="B28">
         <v>9</v>
@@ -948,12 +948,12 @@
         </is>
       </c>
       <c r="E28">
-        <v>0.009119066474791611</v>
+        <v>0.008641955937705392</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>0.00607916020306052</v>
+        <v>0.01152028340455058</v>
       </c>
       <c r="B29">
         <v>10</v>
@@ -969,12 +969,12 @@
         </is>
       </c>
       <c r="E29">
-        <v>0.01519822667785213</v>
+        <v>0.02016223934225598</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>0.02127738688091265</v>
+        <v>0.04622234774589128</v>
       </c>
       <c r="B30">
         <v>11</v>
@@ -990,12 +990,12 @@
         </is>
       </c>
       <c r="E30">
-        <v>0.03647561355876478</v>
+        <v>0.06638458708814725</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>0.06296454790853144</v>
+        <v>0.1590733563808737</v>
       </c>
       <c r="B31">
         <v>12</v>
@@ -1011,12 +1011,12 @@
         </is>
       </c>
       <c r="E31">
-        <v>0.09944016146729621</v>
+        <v>0.225457943469021</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>0.08436000840214437</v>
+        <v>0.117205982597538</v>
       </c>
       <c r="B32">
         <v>13</v>
@@ -1032,12 +1032,12 @@
         </is>
       </c>
       <c r="E32">
-        <v>0.1838001698694406</v>
+        <v>0.3426639260665589</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>0.09063617540650593</v>
+        <v>0.08159561503982761</v>
       </c>
       <c r="B33">
         <v>14</v>
@@ -1053,12 +1053,12 @@
         </is>
       </c>
       <c r="E33">
-        <v>0.2744363452759465</v>
+        <v>0.4242595411063865</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>0.1464941269793639</v>
+        <v>0.07127826679707182</v>
       </c>
       <c r="B34">
         <v>15</v>
@@ -1074,12 +1074,12 @@
         </is>
       </c>
       <c r="E34">
-        <v>0.4209304722553104</v>
+        <v>0.4955378079034584</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>0.1527833407917586</v>
+        <v>0.132530330528228</v>
       </c>
       <c r="B35">
         <v>16</v>
@@ -1095,12 +1095,12 @@
         </is>
       </c>
       <c r="E35">
-        <v>0.573713813047069</v>
+        <v>0.6280681384316864</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>0.1597177192613941</v>
+        <v>0.1286443269403431</v>
       </c>
       <c r="B36">
         <v>17</v>
@@ -1116,12 +1116,12 @@
         </is>
       </c>
       <c r="E36">
-        <v>0.7334315323084631</v>
+        <v>0.7567124653720295</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>0.06744025540431406</v>
+        <v>0.07997252426355089</v>
       </c>
       <c r="B37">
         <v>18</v>
@@ -1137,12 +1137,12 @@
         </is>
       </c>
       <c r="E37">
-        <v>0.8008717877127771</v>
+        <v>0.8366849896355805</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>0.03212776478170733</v>
+        <v>0.0370504029832792</v>
       </c>
       <c r="B38">
         <v>19</v>
@@ -1158,12 +1158,12 @@
         </is>
       </c>
       <c r="E38">
-        <v>0.8329995524944844</v>
+        <v>0.8737353926188596</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>0.05715806599336439</v>
+        <v>0.04243920383126132</v>
       </c>
       <c r="B39">
         <v>20</v>
@@ -1179,12 +1179,12 @@
         </is>
       </c>
       <c r="E39">
-        <v>0.8901576184878489</v>
+        <v>0.9161745964501209</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>0.04974943605172277</v>
+        <v>0.05437789946600139</v>
       </c>
       <c r="B40">
         <v>21</v>
@@ -1200,12 +1200,12 @@
         </is>
       </c>
       <c r="E40">
-        <v>0.9399070545395717</v>
+        <v>0.9705524959161224</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>0.01471353775941947</v>
+        <v>0.00867508023926206</v>
       </c>
       <c r="B41">
         <v>22</v>
@@ -1221,12 +1221,12 @@
         </is>
       </c>
       <c r="E41">
-        <v>0.9546205922989911</v>
+        <v>0.9792275761553844</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>0.0109965021507663</v>
+        <v>0.006895084876664279</v>
       </c>
       <c r="B42">
         <v>23</v>
@@ -1242,12 +1242,12 @@
         </is>
       </c>
       <c r="E42">
-        <v>0.9656170944497574</v>
+        <v>0.9861226610320487</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>0.01491380626272879</v>
+        <v>0.006581275704022162</v>
       </c>
       <c r="B43">
         <v>24</v>
@@ -1263,12 +1263,12 @@
         </is>
       </c>
       <c r="E43">
-        <v>0.9805309007124862</v>
+        <v>0.9927039367360708</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>0.002587182032979721</v>
+        <v>0.001659701846418304</v>
       </c>
       <c r="B44">
         <v>25</v>
@@ -1284,12 +1284,12 @@
         </is>
       </c>
       <c r="E44">
-        <v>0.983118082745466</v>
+        <v>0.9943636385824891</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>0.003492630510482458</v>
+        <v>0.001208165314672148</v>
       </c>
       <c r="B45">
         <v>26</v>
@@ -1305,12 +1305,12 @@
         </is>
       </c>
       <c r="E45">
-        <v>0.9866107132559484</v>
+        <v>0.9955718038971613</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>0.009400225187906652</v>
+        <v>0.003692487931422235</v>
       </c>
       <c r="B46">
         <v>27</v>
@@ -1326,12 +1326,12 @@
         </is>
       </c>
       <c r="E46">
-        <v>0.996010938443855</v>
+        <v>0.9992642918285836</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>0.0004853412588343199</v>
+        <v>8.542583033035389e-05</v>
       </c>
       <c r="B47">
         <v>28</v>
@@ -1347,12 +1347,12 @@
         </is>
       </c>
       <c r="E47">
-        <v>0.9964962797026894</v>
+        <v>0.9993497176589139</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>0.003489368808474163</v>
+        <v>0.0006485389567937071</v>
       </c>
       <c r="B48">
         <v>29</v>
@@ -1368,12 +1368,12 @@
         </is>
       </c>
       <c r="E48">
-        <v>0.9999856485111636</v>
+        <v>0.9999982566157076</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>1.435148883649871e-05</v>
+        <v>1.743384292456202e-06</v>
       </c>
       <c r="B49">
         <v>30</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>0.005865397100194763</v>
+        <v>0.008077789178654803</v>
       </c>
       <c r="B52">
         <v>8</v>
@@ -1452,12 +1452,12 @@
         </is>
       </c>
       <c r="E52">
-        <v>0.005865397100194763</v>
+        <v>0.008077789178654803</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>0.007541224843107553</v>
+        <v>0.006443408418438202</v>
       </c>
       <c r="B53">
         <v>9</v>
@@ -1473,12 +1473,12 @@
         </is>
       </c>
       <c r="E53">
-        <v>0.01340662194330232</v>
+        <v>0.014521197597093</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>0.01675741181562432</v>
+        <v>0.03301127768634121</v>
       </c>
       <c r="B54">
         <v>10</v>
@@ -1494,12 +1494,12 @@
         </is>
       </c>
       <c r="E54">
-        <v>0.03016403375892664</v>
+        <v>0.04753247528343422</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>0.01256870807184592</v>
+        <v>0.02838129735859278</v>
       </c>
       <c r="B55">
         <v>11</v>
@@ -1515,12 +1515,12 @@
         </is>
       </c>
       <c r="E55">
-        <v>0.04273274183077256</v>
+        <v>0.07591377264202699</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>0.04189482795931616</v>
+        <v>0.1100222890971653</v>
       </c>
       <c r="B56">
         <v>12</v>
@@ -1536,12 +1536,12 @@
         </is>
       </c>
       <c r="E56">
-        <v>0.08462756979008873</v>
+        <v>0.1859360617391923</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>0.1056013849816057</v>
+        <v>0.1525093024270095</v>
       </c>
       <c r="B57">
         <v>13</v>
@@ -1557,12 +1557,12 @@
         </is>
       </c>
       <c r="E57">
-        <v>0.1902289547716944</v>
+        <v>0.3384453641662019</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>0.1094706773425665</v>
+        <v>0.1024426187738012</v>
       </c>
       <c r="B58">
         <v>14</v>
@@ -1578,12 +1578,12 @@
         </is>
       </c>
       <c r="E58">
-        <v>0.299699632114261</v>
+        <v>0.4408879829400031</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>0.1087747240856957</v>
+        <v>0.05501573550577428</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -1599,12 +1599,12 @@
         </is>
       </c>
       <c r="E59">
-        <v>0.4084743561999567</v>
+        <v>0.4959037184457774</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>0.1510798528457044</v>
+        <v>0.1362274727469304</v>
       </c>
       <c r="B60">
         <v>16</v>
@@ -1620,12 +1620,12 @@
         </is>
       </c>
       <c r="E60">
-        <v>0.5595542090456611</v>
+        <v>0.6321311911927078</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>0.1568491668470028</v>
+        <v>0.1313220349876847</v>
       </c>
       <c r="B61">
         <v>17</v>
@@ -1641,12 +1641,12 @@
         </is>
       </c>
       <c r="E61">
-        <v>0.7164033758926639</v>
+        <v>0.7634532261803925</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>0.1279385414412465</v>
+        <v>0.1577016750107314</v>
       </c>
       <c r="B62">
         <v>18</v>
@@ -1662,12 +1662,12 @@
         </is>
       </c>
       <c r="E62">
-        <v>0.8443419173339104</v>
+        <v>0.9211549011911239</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>0.07565808266608959</v>
+        <v>0.03511393608010302</v>
       </c>
       <c r="B63">
         <v>19</v>
@@ -1683,12 +1683,12 @@
         </is>
       </c>
       <c r="E63">
-        <v>0.9199999999999999</v>
+        <v>0.9562688372712269</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>0.02828478684267475</v>
+        <v>0.01475763189246142</v>
       </c>
       <c r="B64">
         <v>20</v>
@@ -1704,12 +1704,12 @@
         </is>
       </c>
       <c r="E64">
-        <v>0.9482847868426747</v>
+        <v>0.9710264691636883</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>0.02308677775373296</v>
+        <v>0.01773257215263096</v>
       </c>
       <c r="B65">
         <v>21</v>
@@ -1725,12 +1725,12 @@
         </is>
       </c>
       <c r="E65">
-        <v>0.9713715645964077</v>
+        <v>0.9887590413163192</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>0.01352261415278078</v>
+        <v>0.005603263252371803</v>
       </c>
       <c r="B66">
         <v>22</v>
@@ -1746,12 +1746,12 @@
         </is>
       </c>
       <c r="E66">
-        <v>0.9848941787491885</v>
+        <v>0.994362304568691</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>0.00776195628651807</v>
+        <v>0.003420263107756652</v>
       </c>
       <c r="B67">
         <v>23</v>
@@ -1767,12 +1767,12 @@
         </is>
       </c>
       <c r="E67">
-        <v>0.9926561350357065</v>
+        <v>0.9977825676764477</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>0.005019692707206232</v>
+        <v>0.001556334487959067</v>
       </c>
       <c r="B68">
         <v>24</v>
@@ -1788,12 +1788,12 @@
         </is>
       </c>
       <c r="E68">
-        <v>0.9976758277429127</v>
+        <v>0.9993389021644068</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>0.0008578229820385198</v>
+        <v>0.000385640404096052</v>
       </c>
       <c r="B69">
         <v>25</v>
@@ -1809,12 +1809,12 @@
         </is>
       </c>
       <c r="E69">
-        <v>0.9985336507249513</v>
+        <v>0.9997245425685028</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>0.0002051504003462454</v>
+        <v>5.050052910781633e-05</v>
       </c>
       <c r="B70">
         <v>26</v>
@@ -1830,12 +1830,12 @@
         </is>
       </c>
       <c r="E70">
-        <v>0.9987388011252976</v>
+        <v>0.9997750430976107</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>0.0004648344514174421</v>
+        <v>0.0001285468013653507</v>
       </c>
       <c r="B71">
         <v>27</v>
@@ -1851,12 +1851,12 @@
         </is>
       </c>
       <c r="E71">
-        <v>0.999203635576715</v>
+        <v>0.999903589898976</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>0.0007418307725600519</v>
+        <v>9.181914383239334e-05</v>
       </c>
       <c r="B72">
         <v>28</v>
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="E72">
-        <v>0.9999454663492751</v>
+        <v>0.9999954090428084</v>
       </c>
     </row>
     <row r="73">
@@ -1893,12 +1893,12 @@
         </is>
       </c>
       <c r="E73">
-        <v>0.9999454663492751</v>
+        <v>0.9999954090428084</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>5.453365072495131e-05</v>
+        <v>4.590957191619666e-06</v>
       </c>
       <c r="B74">
         <v>30</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>0.0004469320010841813</v>
+        <v>0.01136230943885825</v>
       </c>
       <c r="B76">
         <v>6</v>
@@ -1956,12 +1956,12 @@
         </is>
       </c>
       <c r="E76">
-        <v>0.0004469320010841813</v>
+        <v>0.01136230943885825</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>0.002026042938934491</v>
+        <v>0.003866363931235809</v>
       </c>
       <c r="B77">
         <v>7</v>
@@ -1977,12 +1977,12 @@
         </is>
       </c>
       <c r="E77">
-        <v>0.002472974940018672</v>
+        <v>0.01522867337009406</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>0.002926494848465582</v>
+        <v>0.003436462985603433</v>
       </c>
       <c r="B78">
         <v>8</v>
@@ -1998,12 +1998,12 @@
         </is>
       </c>
       <c r="E78">
-        <v>0.005399469788484254</v>
+        <v>0.0186651363556975</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>0.004727398667527766</v>
+        <v>0.003444447216746925</v>
       </c>
       <c r="B79">
         <v>9</v>
@@ -2019,12 +2019,12 @@
         </is>
       </c>
       <c r="E79">
-        <v>0.01012686845601202</v>
+        <v>0.02210958357244442</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>0.01598309982164548</v>
+        <v>0.02684822475610669</v>
       </c>
       <c r="B80">
         <v>10</v>
@@ -2040,12 +2040,12 @@
         </is>
       </c>
       <c r="E80">
-        <v>0.0261099682776575</v>
+        <v>0.04895780832855111</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>0.05562891719063187</v>
+        <v>0.1071191896005389</v>
       </c>
       <c r="B81">
         <v>11</v>
@@ -2061,12 +2061,12 @@
         </is>
       </c>
       <c r="E81">
-        <v>0.08173888546828936</v>
+        <v>0.15607699792909</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>0.09486743457266859</v>
+        <v>0.2124479153671499</v>
       </c>
       <c r="B82">
         <v>12</v>
@@ -2082,12 +2082,12 @@
         </is>
       </c>
       <c r="E82">
-        <v>0.176606320040958</v>
+        <v>0.3685249132962399</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>0.1319367527430791</v>
+        <v>0.1624840939145188</v>
       </c>
       <c r="B83">
         <v>13</v>
@@ -2103,12 +2103,12 @@
         </is>
       </c>
       <c r="E83">
-        <v>0.3085430727840371</v>
+        <v>0.5310090072107587</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>0.1589832495658255</v>
+        <v>0.1268671873050725</v>
       </c>
       <c r="B84">
         <v>14</v>
@@ -2124,12 +2124,12 @@
         </is>
       </c>
       <c r="E84">
-        <v>0.4675263223498626</v>
+        <v>0.6578761945158312</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>0.1696053613435818</v>
+        <v>0.07314903066443773</v>
       </c>
       <c r="B85">
         <v>15</v>
@@ -2145,12 +2145,12 @@
         </is>
       </c>
       <c r="E85">
-        <v>0.6371316836934444</v>
+        <v>0.731025225180269</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>0.1368970287073815</v>
+        <v>0.105260610294668</v>
       </c>
       <c r="B86">
         <v>16</v>
@@ -2166,12 +2166,12 @@
         </is>
       </c>
       <c r="E86">
-        <v>0.7740287124008258</v>
+        <v>0.836285835474937</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>0.0867726741131631</v>
+        <v>0.06195164550013723</v>
       </c>
       <c r="B87">
         <v>17</v>
@@ -2187,12 +2187,12 @@
         </is>
       </c>
       <c r="E87">
-        <v>0.860801386513989</v>
+        <v>0.8982374809750743</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>0.04753060135254967</v>
+        <v>0.04997130666932808</v>
       </c>
       <c r="B88">
         <v>18</v>
@@ -2208,12 +2208,12 @@
         </is>
       </c>
       <c r="E88">
-        <v>0.9083319878665387</v>
+        <v>0.9482087876444023</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>0.02966796110332181</v>
+        <v>0.01506424810998278</v>
       </c>
       <c r="B89">
         <v>19</v>
@@ -2229,12 +2229,12 @@
         </is>
       </c>
       <c r="E89">
-        <v>0.9379999489698605</v>
+        <v>0.9632730357543851</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>0.01392579046522756</v>
+        <v>0.008616981461613315</v>
       </c>
       <c r="B90">
         <v>20</v>
@@ -2250,12 +2250,12 @@
         </is>
       </c>
       <c r="E90">
-        <v>0.951925739435088</v>
+        <v>0.9718900172159984</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>0.0144987292658687</v>
+        <v>0.01320716584745128</v>
       </c>
       <c r="B91">
         <v>21</v>
@@ -2271,12 +2271,12 @@
         </is>
       </c>
       <c r="E91">
-        <v>0.9664244687009567</v>
+        <v>0.9850971830634497</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>0.01093111600405564</v>
+        <v>0.005371141994560742</v>
       </c>
       <c r="B92">
         <v>22</v>
@@ -2292,12 +2292,12 @@
         </is>
       </c>
       <c r="E92">
-        <v>0.9773555847050124</v>
+        <v>0.9904683250580104</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>0.007877045806661022</v>
+        <v>0.004115621647246688</v>
       </c>
       <c r="B93">
         <v>23</v>
@@ -2313,12 +2313,12 @@
         </is>
       </c>
       <c r="E93">
-        <v>0.9852326305116734</v>
+        <v>0.9945839467052571</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>0.004445582630344362</v>
+        <v>0.001634771326629906</v>
       </c>
       <c r="B94">
         <v>24</v>
@@ -2334,12 +2334,12 @@
         </is>
       </c>
       <c r="E94">
-        <v>0.9896782131420178</v>
+        <v>0.996218718031887</v>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>0.00418238004570962</v>
+        <v>0.002235335212954415</v>
       </c>
       <c r="B95">
         <v>25</v>
@@ -2355,12 +2355,12 @@
         </is>
       </c>
       <c r="E95">
-        <v>0.9938605931877273</v>
+        <v>0.9984540532448415</v>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>0.00291582871273545</v>
+        <v>0.0008408393422989596</v>
       </c>
       <c r="B96">
         <v>26</v>
@@ -2376,12 +2376,12 @@
         </is>
       </c>
       <c r="E96">
-        <v>0.9967764219004628</v>
+        <v>0.9992948925871404</v>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>0.001467430222558333</v>
+        <v>0.0004803014047256668</v>
       </c>
       <c r="B97">
         <v>27</v>
@@ -2397,12 +2397,12 @@
         </is>
       </c>
       <c r="E97">
-        <v>0.9982438521230211</v>
+        <v>0.9997751939918661</v>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>0.0007577139166719649</v>
+        <v>0.0001105316998927119</v>
       </c>
       <c r="B98">
         <v>28</v>
@@ -2418,12 +2418,12 @@
         </is>
       </c>
       <c r="E98">
-        <v>0.9990015660396931</v>
+        <v>0.9998857256917588</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>0.0002535821484859943</v>
+        <v>3.917263404775568e-05</v>
       </c>
       <c r="B99">
         <v>29</v>
@@ -2439,12 +2439,12 @@
         </is>
       </c>
       <c r="E99">
-        <v>0.9992551481881791</v>
+        <v>0.9999248983258066</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>0.0005447049119437296</v>
+        <v>6.187779136205994e-05</v>
       </c>
       <c r="B100">
         <v>30</v>
@@ -2460,12 +2460,12 @@
         </is>
       </c>
       <c r="E100">
-        <v>0.9997998531001229</v>
+        <v>0.9999867761171686</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>0.000200146899877193</v>
+        <v>1.322388283140797e-05</v>
       </c>
       <c r="B101">
         <v>31</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>0.0009217479252559566</v>
+        <v>0.02260267523669732</v>
       </c>
       <c r="B102">
         <v>6</v>
@@ -2502,12 +2502,12 @@
         </is>
       </c>
       <c r="E102">
-        <v>0.0009217479252559566</v>
+        <v>0.02260267523669732</v>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>0.0006059397472984363</v>
+        <v>0.001129371864894339</v>
       </c>
       <c r="B103">
         <v>7</v>
@@ -2523,12 +2523,12 @@
         </is>
       </c>
       <c r="E103">
-        <v>0.001527687672554393</v>
+        <v>0.02373204710159166</v>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>0.001211879494596873</v>
+        <v>0.001390020818232402</v>
       </c>
       <c r="B104">
         <v>8</v>
@@ -2544,12 +2544,12 @@
         </is>
       </c>
       <c r="E104">
-        <v>0.002739567167151266</v>
+        <v>0.02512206791982406</v>
       </c>
     </row>
     <row r="105">
       <c r="A105">
-        <v>0.004544407024471149</v>
+        <v>0.003234292612374586</v>
       </c>
       <c r="B105">
         <v>9</v>
@@ -2565,12 +2565,12 @@
         </is>
       </c>
       <c r="E105">
-        <v>0.007283974191622414</v>
+        <v>0.02835636053219865</v>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>0.02590325406573931</v>
+        <v>0.0425018193296943</v>
       </c>
       <c r="B106">
         <v>10</v>
@@ -2586,12 +2586,12 @@
         </is>
       </c>
       <c r="E106">
-        <v>0.03318722825736173</v>
+        <v>0.07085817986189295</v>
       </c>
     </row>
     <row r="107">
       <c r="A107">
-        <v>0.0594490378219972</v>
+        <v>0.1118171177871818</v>
       </c>
       <c r="B107">
         <v>11</v>
@@ -2607,12 +2607,12 @@
         </is>
       </c>
       <c r="E107">
-        <v>0.09263626607935892</v>
+        <v>0.1826752976490748</v>
       </c>
     </row>
     <row r="108">
       <c r="A108">
-        <v>0.1114900918975698</v>
+        <v>0.2438758322922079</v>
       </c>
       <c r="B108">
         <v>12</v>
@@ -2628,12 +2628,12 @@
         </is>
       </c>
       <c r="E108">
-        <v>0.2041263579769287</v>
+        <v>0.4265511299412826</v>
       </c>
     </row>
     <row r="109">
       <c r="A109">
-        <v>0.1148227605077112</v>
+        <v>0.1381240557490417</v>
       </c>
       <c r="B109">
         <v>13</v>
@@ -2649,12 +2649,12 @@
         </is>
       </c>
       <c r="E109">
-        <v>0.3189491184846399</v>
+        <v>0.5646751856903244</v>
       </c>
     </row>
     <row r="110">
       <c r="A110">
-        <v>0.1452843180042334</v>
+        <v>0.1132433888598477</v>
       </c>
       <c r="B110">
         <v>14</v>
@@ -2670,12 +2670,12 @@
         </is>
       </c>
       <c r="E110">
-        <v>0.4642334364888733</v>
+        <v>0.677918574550172</v>
       </c>
     </row>
     <row r="111">
       <c r="A111">
-        <v>0.14307958612975</v>
+        <v>0.06027583235636759</v>
       </c>
       <c r="B111">
         <v>15</v>
@@ -2691,12 +2691,12 @@
         </is>
       </c>
       <c r="E111">
-        <v>0.6073130226186233</v>
+        <v>0.7381944069065396</v>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>0.1417128005018507</v>
+        <v>0.1064333134063867</v>
       </c>
       <c r="B112">
         <v>16</v>
@@ -2712,12 +2712,12 @@
         </is>
       </c>
       <c r="E112">
-        <v>0.7490258231204741</v>
+        <v>0.8446277203129263</v>
       </c>
     </row>
     <row r="113">
       <c r="A113">
-        <v>0.1201967195028726</v>
+        <v>0.08383144016646887</v>
       </c>
       <c r="B113">
         <v>17</v>
@@ -2733,12 +2733,12 @@
         </is>
       </c>
       <c r="E113">
-        <v>0.8692225426233466</v>
+        <v>0.9284591604793953</v>
       </c>
     </row>
     <row r="114">
       <c r="A114">
-        <v>0.05077746866307472</v>
+        <v>0.03814425002794958</v>
       </c>
       <c r="B114">
         <v>18</v>
@@ -2754,12 +2754,12 @@
         </is>
       </c>
       <c r="E114">
-        <v>0.9200000112864214</v>
+        <v>0.9666034105073448</v>
       </c>
     </row>
     <row r="115">
       <c r="A115">
-        <v>0.03085707602540489</v>
+        <v>0.01304656281022238</v>
       </c>
       <c r="B115">
         <v>19</v>
@@ -2775,12 +2775,12 @@
         </is>
       </c>
       <c r="E115">
-        <v>0.9508570873118263</v>
+        <v>0.9796499733175672</v>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>0.01812429975691164</v>
+        <v>0.007531712155656668</v>
       </c>
       <c r="B116">
         <v>20</v>
@@ -2796,12 +2796,12 @@
         </is>
       </c>
       <c r="E116">
-        <v>0.9689813870687379</v>
+        <v>0.9871816854732238</v>
       </c>
     </row>
     <row r="117">
       <c r="A117">
-        <v>0.01095248437765297</v>
+        <v>0.006700201894669272</v>
       </c>
       <c r="B117">
         <v>21</v>
@@ -2817,12 +2817,12 @@
         </is>
       </c>
       <c r="E117">
-        <v>0.9799338714463909</v>
+        <v>0.9938818873678931</v>
       </c>
     </row>
     <row r="118">
       <c r="A118">
-        <v>0.007377510408725758</v>
+        <v>0.002434541423855458</v>
       </c>
       <c r="B118">
         <v>22</v>
@@ -2838,12 +2838,12 @@
         </is>
       </c>
       <c r="E118">
-        <v>0.9873113818551166</v>
+        <v>0.9963164287917485</v>
       </c>
     </row>
     <row r="119">
       <c r="A119">
-        <v>0.002539021567434216</v>
+        <v>0.0008908580226705242</v>
       </c>
       <c r="B119">
         <v>23</v>
@@ -2859,12 +2859,12 @@
         </is>
       </c>
       <c r="E119">
-        <v>0.9898504034225508</v>
+        <v>0.9972072868144191</v>
       </c>
     </row>
     <row r="120">
       <c r="A120">
-        <v>0.004610150428951025</v>
+        <v>0.001138514628180659</v>
       </c>
       <c r="B120">
         <v>24</v>
@@ -2880,12 +2880,12 @@
         </is>
       </c>
       <c r="E120">
-        <v>0.9944605538515019</v>
+        <v>0.9983458014425998</v>
       </c>
     </row>
     <row r="121">
       <c r="A121">
-        <v>0.004000754215108046</v>
+        <v>0.001436055433375802</v>
       </c>
       <c r="B121">
         <v>25</v>
@@ -2901,12 +2901,12 @@
         </is>
       </c>
       <c r="E121">
-        <v>0.9984613080666099</v>
+        <v>0.9997818568759755</v>
       </c>
     </row>
     <row r="122">
       <c r="A122">
-        <v>0.0008156555643785587</v>
+        <v>0.0001579933655618413</v>
       </c>
       <c r="B122">
         <v>26</v>
@@ -2922,12 +2922,12 @@
         </is>
       </c>
       <c r="E122">
-        <v>0.9992769636309885</v>
+        <v>0.9999398502415374</v>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>4.359380254137761e-05</v>
+        <v>9.623961354020786e-06</v>
       </c>
       <c r="B123">
         <v>27</v>
@@ -2943,7 +2943,7 @@
         </is>
       </c>
       <c r="E123">
-        <v>0.9993205574335299</v>
+        <v>0.9999494742028914</v>
       </c>
     </row>
     <row r="124">
@@ -2964,12 +2964,12 @@
         </is>
       </c>
       <c r="E124">
-        <v>0.9993205574335299</v>
+        <v>0.9999494742028914</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>0.0002181100929740122</v>
+        <v>2.261630918194885e-05</v>
       </c>
       <c r="B125">
         <v>29</v>
@@ -2985,12 +2985,12 @@
         </is>
       </c>
       <c r="E125">
-        <v>0.9995386675265039</v>
+        <v>0.9999720905120734</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>0.000230666236748066</v>
+        <v>1.764392914903811e-05</v>
       </c>
       <c r="B126">
         <v>30</v>
@@ -3006,12 +3006,12 @@
         </is>
       </c>
       <c r="E126">
-        <v>0.9997693337632519</v>
+        <v>0.9999897344412224</v>
       </c>
     </row>
     <row r="127">
       <c r="A127">
-        <v>0.000230666236748066</v>
+        <v>1.026555877762217e-05</v>
       </c>
       <c r="B127">
         <v>31</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="128">
       <c r="A128">
-        <v>0.007403190136094685</v>
+        <v>0.01428798816512645</v>
       </c>
       <c r="B128">
         <v>7</v>
@@ -3048,12 +3048,12 @@
         </is>
       </c>
       <c r="E128">
-        <v>0.007403190136094685</v>
+        <v>0.01428798816512645</v>
       </c>
     </row>
     <row r="129">
       <c r="A129">
-        <v>0.007478349426816459</v>
+        <v>0.008880836680617586</v>
       </c>
       <c r="B129">
         <v>8</v>
@@ -3069,12 +3069,12 @@
         </is>
       </c>
       <c r="E129">
-        <v>0.01488153956291114</v>
+        <v>0.02316882484574403</v>
       </c>
     </row>
     <row r="130">
       <c r="A130">
-        <v>0.01121752414022469</v>
+        <v>0.00826287651095943</v>
       </c>
       <c r="B130">
         <v>9</v>
@@ -3090,12 +3090,12 @@
         </is>
       </c>
       <c r="E130">
-        <v>0.02609906370313583</v>
+        <v>0.03143170135670346</v>
       </c>
     </row>
     <row r="131">
       <c r="A131">
-        <v>0.02243504828044938</v>
+        <v>0.03810754379558626</v>
       </c>
       <c r="B131">
         <v>10</v>
@@ -3111,12 +3111,12 @@
         </is>
       </c>
       <c r="E131">
-        <v>0.04853411198358521</v>
+        <v>0.06953924515228972</v>
       </c>
     </row>
     <row r="132">
       <c r="A132">
-        <v>0.04487009656089876</v>
+        <v>0.08736645974364016</v>
       </c>
       <c r="B132">
         <v>11</v>
@@ -3132,12 +3132,12 @@
         </is>
       </c>
       <c r="E132">
-        <v>0.09340420854448397</v>
+        <v>0.1569057048959299</v>
       </c>
     </row>
     <row r="133">
       <c r="A133">
-        <v>0.0859972604438532</v>
+        <v>0.1947417207381815</v>
       </c>
       <c r="B133">
         <v>12</v>
@@ -3153,12 +3153,12 @@
         </is>
       </c>
       <c r="E133">
-        <v>0.1794014689883372</v>
+        <v>0.3516474256341114</v>
       </c>
     </row>
     <row r="134">
       <c r="A134">
-        <v>0.145827813822921</v>
+        <v>0.1816007041000721</v>
       </c>
       <c r="B134">
         <v>13</v>
@@ -3174,12 +3174,12 @@
         </is>
       </c>
       <c r="E134">
-        <v>0.3252292828112581</v>
+        <v>0.5332481297341835</v>
       </c>
     </row>
     <row r="135">
       <c r="A135">
-        <v>0.2213196844061383</v>
+        <v>0.1785858075147702</v>
       </c>
       <c r="B135">
         <v>14</v>
@@ -3195,12 +3195,12 @@
         </is>
       </c>
       <c r="E135">
-        <v>0.5465489672173963</v>
+        <v>0.7118339372489537</v>
       </c>
     </row>
     <row r="136">
       <c r="A136">
-        <v>0.2223362138131502</v>
+        <v>0.09696356843908879</v>
       </c>
       <c r="B136">
         <v>15</v>
@@ -3216,12 +3216,12 @@
         </is>
       </c>
       <c r="E136">
-        <v>0.7688851810305466</v>
+        <v>0.8087975056880424</v>
       </c>
     </row>
     <row r="137">
       <c r="A137">
-        <v>0.1061136446055359</v>
+        <v>0.08250236416580059</v>
       </c>
       <c r="B137">
         <v>16</v>
@@ -3237,12 +3237,12 @@
         </is>
       </c>
       <c r="E137">
-        <v>0.8749988256360824</v>
+        <v>0.891299869853843</v>
       </c>
     </row>
     <row r="138">
       <c r="A138">
-        <v>0.04981557789039145</v>
+        <v>0.03596340926752994</v>
       </c>
       <c r="B138">
         <v>17</v>
@@ -3258,12 +3258,12 @@
         </is>
       </c>
       <c r="E138">
-        <v>0.9248144035264739</v>
+        <v>0.927263279121373</v>
       </c>
     </row>
     <row r="139">
       <c r="A139">
-        <v>0.03672282944665851</v>
+        <v>0.03902980253363669</v>
       </c>
       <c r="B139">
         <v>18</v>
@@ -3279,12 +3279,12 @@
         </is>
       </c>
       <c r="E139">
-        <v>0.9615372329731324</v>
+        <v>0.9662930816550097</v>
       </c>
     </row>
     <row r="140">
       <c r="A140">
-        <v>0.02040950539549758</v>
+        <v>0.01859498328698632</v>
       </c>
       <c r="B140">
         <v>19</v>
@@ -3300,12 +3300,12 @@
         </is>
       </c>
       <c r="E140">
-        <v>0.98194673836863</v>
+        <v>0.984888064941996</v>
       </c>
     </row>
     <row r="141">
       <c r="A141">
-        <v>0.007006724877537331</v>
+        <v>0.00627323202531764</v>
       </c>
       <c r="B141">
         <v>20</v>
@@ -3321,12 +3321,12 @@
         </is>
       </c>
       <c r="E141">
-        <v>0.9889534632461674</v>
+        <v>0.9911612969673137</v>
       </c>
     </row>
     <row r="142">
       <c r="A142">
-        <v>0.002529110132787677</v>
+        <v>0.003333239703004597</v>
       </c>
       <c r="B142">
         <v>21</v>
@@ -3342,12 +3342,12 @@
         </is>
       </c>
       <c r="E142">
-        <v>0.9914825733789551</v>
+        <v>0.9944945366703183</v>
       </c>
     </row>
     <row r="143">
       <c r="A143">
-        <v>0.005997711399597522</v>
+        <v>0.004264861473928635</v>
       </c>
       <c r="B143">
         <v>22</v>
@@ -3363,12 +3363,12 @@
         </is>
       </c>
       <c r="E143">
-        <v>0.9974802847785526</v>
+        <v>0.9987593981442469</v>
       </c>
     </row>
     <row r="144">
       <c r="A144">
-        <v>4.885353896915275e-05</v>
+        <v>3.745213149443368e-05</v>
       </c>
       <c r="B144">
         <v>23</v>
@@ -3384,12 +3384,12 @@
         </is>
       </c>
       <c r="E144">
-        <v>0.9975291383175217</v>
+        <v>0.9987968502757413</v>
       </c>
     </row>
     <row r="145">
       <c r="A145">
-        <v>0.0004791404783513058</v>
+        <v>0.0002528018875874273</v>
       </c>
       <c r="B145">
         <v>24</v>
@@ -3405,12 +3405,12 @@
         </is>
       </c>
       <c r="E145">
-        <v>0.9980082787958729</v>
+        <v>0.9990496521633287</v>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>0.0003363378259799362</v>
+        <v>0.0002574834040242315</v>
       </c>
       <c r="B146">
         <v>25</v>
@@ -3426,12 +3426,12 @@
         </is>
       </c>
       <c r="E146">
-        <v>0.9983446166218529</v>
+        <v>0.999307135567353</v>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>0.00165538337814706</v>
+        <v>0.000692864432647023</v>
       </c>
       <c r="B147">
         <v>26</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="153">
       <c r="A153">
-        <v>0.02860161267339187</v>
+        <v>0.3427245183736425</v>
       </c>
       <c r="B153">
         <v>6</v>
@@ -3573,12 +3573,12 @@
         </is>
       </c>
       <c r="E153">
-        <v>0.02860161267339187</v>
+        <v>0.3427245183736425</v>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>0.04916934053352857</v>
+        <v>0.04353145105211304</v>
       </c>
       <c r="B154">
         <v>7</v>
@@ -3594,12 +3594,12 @@
         </is>
       </c>
       <c r="E154">
-        <v>0.07777095320692044</v>
+        <v>0.3862559694257556</v>
       </c>
     </row>
     <row r="155">
       <c r="A155">
-        <v>0.05443976551866465</v>
+        <v>0.02965755632969766</v>
       </c>
       <c r="B155">
         <v>8</v>
@@ -3615,12 +3615,12 @@
         </is>
       </c>
       <c r="E155">
-        <v>0.1322107187255851</v>
+        <v>0.4159135257554533</v>
       </c>
     </row>
     <row r="156">
       <c r="A156">
-        <v>0.07064217027904851</v>
+        <v>0.0238799498068327</v>
       </c>
       <c r="B156">
         <v>9</v>
@@ -3636,12 +3636,12 @@
         </is>
       </c>
       <c r="E156">
-        <v>0.2028528890046336</v>
+        <v>0.4397934755622859</v>
       </c>
     </row>
     <row r="157">
       <c r="A157">
-        <v>0.1264105978487861</v>
+        <v>0.09851476305971617</v>
       </c>
       <c r="B157">
         <v>10</v>
@@ -3657,12 +3657,12 @@
         </is>
       </c>
       <c r="E157">
-        <v>0.3292634868534197</v>
+        <v>0.5383082386220021</v>
       </c>
     </row>
     <row r="158">
       <c r="A158">
-        <v>0.2196036616825461</v>
+        <v>0.1961858585132353</v>
       </c>
       <c r="B158">
         <v>11</v>
@@ -3678,12 +3678,12 @@
         </is>
       </c>
       <c r="E158">
-        <v>0.5488671485359657</v>
+        <v>0.7344940971352374</v>
       </c>
     </row>
     <row r="159">
       <c r="A159">
-        <v>0.138486484892857</v>
+        <v>0.1438818371058719</v>
       </c>
       <c r="B159">
         <v>12</v>
@@ -3699,12 +3699,12 @@
         </is>
       </c>
       <c r="E159">
-        <v>0.6873536334288227</v>
+        <v>0.8783759342411092</v>
       </c>
     </row>
     <row r="160">
       <c r="A160">
-        <v>0.07486106538648636</v>
+        <v>0.04277203786730715</v>
       </c>
       <c r="B160">
         <v>13</v>
@@ -3720,12 +3720,12 @@
         </is>
       </c>
       <c r="E160">
-        <v>0.7622146988153091</v>
+        <v>0.9211479721084164</v>
       </c>
     </row>
     <row r="161">
       <c r="A161">
-        <v>0.06061824060379435</v>
+        <v>0.02244200768175645</v>
       </c>
       <c r="B161">
         <v>14</v>
@@ -3741,12 +3741,12 @@
         </is>
       </c>
       <c r="E161">
-        <v>0.8228329394191034</v>
+        <v>0.9435899797901728</v>
       </c>
     </row>
     <row r="162">
       <c r="A162">
-        <v>0.06406273800690865</v>
+        <v>0.01281790597431251</v>
       </c>
       <c r="B162">
         <v>15</v>
@@ -3762,12 +3762,12 @@
         </is>
       </c>
       <c r="E162">
-        <v>0.8868956774260121</v>
+        <v>0.9564078857644853</v>
       </c>
     </row>
     <row r="163">
       <c r="A163">
-        <v>0.03310353638342513</v>
+        <v>0.0118090997021887</v>
       </c>
       <c r="B163">
         <v>16</v>
@@ -3783,12 +3783,12 @@
         </is>
       </c>
       <c r="E163">
-        <v>0.9199992138094373</v>
+        <v>0.968216985466674</v>
       </c>
     </row>
     <row r="164">
       <c r="A164">
-        <v>0.0329806941079931</v>
+        <v>0.01092386658143864</v>
       </c>
       <c r="B164">
         <v>17</v>
@@ -3804,12 +3804,12 @@
         </is>
       </c>
       <c r="E164">
-        <v>0.9529799079174304</v>
+        <v>0.9791408520481126</v>
       </c>
     </row>
     <row r="165">
       <c r="A165">
-        <v>0.01699743996698</v>
+        <v>0.00828951167260754</v>
       </c>
       <c r="B165">
         <v>18</v>
@@ -3825,12 +3825,12 @@
         </is>
       </c>
       <c r="E165">
-        <v>0.9699773478844104</v>
+        <v>0.9874303637207202</v>
       </c>
     </row>
     <row r="166">
       <c r="A166">
-        <v>0.01710652390756364</v>
+        <v>0.007150391895398698</v>
       </c>
       <c r="B166">
         <v>19</v>
@@ -3846,12 +3846,12 @@
         </is>
       </c>
       <c r="E166">
-        <v>0.987083871791974</v>
+        <v>0.9945807556161189</v>
       </c>
     </row>
     <row r="167">
       <c r="A167">
-        <v>0.008827937281647855</v>
+        <v>0.003626310296676669</v>
       </c>
       <c r="B167">
         <v>20</v>
@@ -3867,12 +3867,12 @@
         </is>
       </c>
       <c r="E167">
-        <v>0.9959118090736219</v>
+        <v>0.9982070659127956</v>
       </c>
     </row>
     <row r="168">
       <c r="A168">
-        <v>0.001907494852908659</v>
+        <v>0.001153723876916648</v>
       </c>
       <c r="B168">
         <v>21</v>
@@ -3888,12 +3888,12 @@
         </is>
       </c>
       <c r="E168">
-        <v>0.9978193039265305</v>
+        <v>0.9993607897897122</v>
       </c>
     </row>
     <row r="169">
       <c r="A169">
-        <v>0.001365023364600787</v>
+        <v>0.0004459867372306807</v>
       </c>
       <c r="B169">
         <v>22</v>
@@ -3909,12 +3909,12 @@
         </is>
       </c>
       <c r="E169">
-        <v>0.9991843272911313</v>
+        <v>0.9998067765269429</v>
       </c>
     </row>
     <row r="170">
       <c r="A170">
-        <v>0.0002476500272709851</v>
+        <v>8.537781367640236e-05</v>
       </c>
       <c r="B170">
         <v>23</v>
@@ -3930,7 +3930,7 @@
         </is>
       </c>
       <c r="E170">
-        <v>0.9994319773184023</v>
+        <v>0.9998921543406193</v>
       </c>
     </row>
     <row r="171">
@@ -3951,12 +3951,12 @@
         </is>
       </c>
       <c r="E171">
-        <v>0.9994319773184023</v>
+        <v>0.9998921543406193</v>
       </c>
     </row>
     <row r="172">
       <c r="A172">
-        <v>1.96547640691258e-06</v>
+        <v>0</v>
       </c>
       <c r="B172">
         <v>25</v>
@@ -3972,12 +3972,12 @@
         </is>
       </c>
       <c r="E172">
-        <v>0.9994339427948091</v>
+        <v>0.9998921543406193</v>
       </c>
     </row>
     <row r="173">
       <c r="A173">
-        <v>0.0005660572051908232</v>
+        <v>0.0001078456593807188</v>
       </c>
       <c r="B173">
         <v>26</v>
@@ -4103,7 +4103,7 @@
     </row>
     <row r="179">
       <c r="A179">
-        <v>0.02778737170141132</v>
+        <v>0.3390634830512376</v>
       </c>
       <c r="B179">
         <v>6</v>
@@ -4119,12 +4119,12 @@
         </is>
       </c>
       <c r="E179">
-        <v>0.02778737170141132</v>
+        <v>0.3390634830512376</v>
       </c>
     </row>
     <row r="180">
       <c r="A180">
-        <v>0.04761911039281185</v>
+        <v>0.04293123820338515</v>
       </c>
       <c r="B180">
         <v>7</v>
@@ -4140,12 +4140,12 @@
         </is>
       </c>
       <c r="E180">
-        <v>0.07540648209422317</v>
+        <v>0.3819947212546227</v>
       </c>
     </row>
     <row r="181">
       <c r="A181">
-        <v>0.05272337071008804</v>
+        <v>0.02924869949514325</v>
       </c>
       <c r="B181">
         <v>8</v>
@@ -4161,12 +4161,12 @@
         </is>
       </c>
       <c r="E181">
-        <v>0.1281298528043112</v>
+        <v>0.4112434207497659</v>
       </c>
     </row>
     <row r="182">
       <c r="A182">
-        <v>0.06841580738799496</v>
+        <v>0.02355103042951187</v>
       </c>
       <c r="B182">
         <v>9</v>
@@ -4182,12 +4182,12 @@
         </is>
       </c>
       <c r="E182">
-        <v>0.1965456601923062</v>
+        <v>0.4347944511792778</v>
       </c>
     </row>
     <row r="183">
       <c r="A183">
-        <v>0.1224264482943175</v>
+        <v>0.09715653628370187</v>
       </c>
       <c r="B183">
         <v>10</v>
@@ -4203,12 +4203,12 @@
         </is>
       </c>
       <c r="E183">
-        <v>0.3189721084866237</v>
+        <v>0.5319509874629798</v>
       </c>
     </row>
     <row r="184">
       <c r="A184">
-        <v>0.2126816876751624</v>
+        <v>0.1934813632666841</v>
       </c>
       <c r="B184">
         <v>11</v>
@@ -4224,12 +4224,12 @@
         </is>
       </c>
       <c r="E184">
-        <v>0.5316537961617861</v>
+        <v>0.7254323507296637</v>
       </c>
     </row>
     <row r="185">
       <c r="A185">
-        <v>0.1341212947314858</v>
+        <v>0.1418977396535056</v>
       </c>
       <c r="B185">
         <v>12</v>
@@ -4245,12 +4245,12 @@
         </is>
       </c>
       <c r="E185">
-        <v>0.6657750908932719</v>
+        <v>0.8673300903831693</v>
       </c>
     </row>
     <row r="186">
       <c r="A186">
-        <v>0.07250106119048436</v>
+        <v>0.04218239292893643</v>
       </c>
       <c r="B186">
         <v>13</v>
@@ -4266,12 +4266,12 @@
         </is>
       </c>
       <c r="E186">
-        <v>0.7382761520837563</v>
+        <v>0.9095124833121058</v>
       </c>
     </row>
     <row r="187">
       <c r="A187">
-        <v>0.05870756226749382</v>
+        <v>0.02213236760937284</v>
       </c>
       <c r="B187">
         <v>14</v>
@@ -4287,12 +4287,12 @@
         </is>
       </c>
       <c r="E187">
-        <v>0.7969837143512501</v>
+        <v>0.9316448509214786</v>
       </c>
     </row>
     <row r="188">
       <c r="A188">
-        <v>0.06204339148569304</v>
+        <v>0.01264136756333727</v>
       </c>
       <c r="B188">
         <v>15</v>
@@ -4308,12 +4308,12 @@
         </is>
       </c>
       <c r="E188">
-        <v>0.8590271058369432</v>
+        <v>0.9442862184848159</v>
       </c>
     </row>
     <row r="189">
       <c r="A189">
-        <v>0.03197281243161583</v>
+        <v>0.0116140070894778</v>
       </c>
       <c r="B189">
         <v>16</v>
@@ -4329,12 +4329,12 @@
         </is>
       </c>
       <c r="E189">
-        <v>0.890999918268559</v>
+        <v>0.9559002255742937</v>
       </c>
     </row>
     <row r="190">
       <c r="A190">
-        <v>0.04493581445380987</v>
+        <v>0.01515644421256157</v>
       </c>
       <c r="B190">
         <v>17</v>
@@ -4350,12 +4350,12 @@
         </is>
       </c>
       <c r="E190">
-        <v>0.9359357327223689</v>
+        <v>0.9710566697868552</v>
       </c>
     </row>
     <row r="191">
       <c r="A191">
-        <v>0.02315899929078201</v>
+        <v>0.01150045268310648</v>
       </c>
       <c r="B191">
         <v>18</v>
@@ -4371,12 +4371,12 @@
         </is>
       </c>
       <c r="E191">
-        <v>0.9590947320131509</v>
+        <v>0.9825571224699617</v>
       </c>
     </row>
     <row r="192">
       <c r="A192">
-        <v>0.02330730230878138</v>
+        <v>0.009921432626943085</v>
       </c>
       <c r="B192">
         <v>19</v>
@@ -4392,12 +4392,12 @@
         </is>
       </c>
       <c r="E192">
-        <v>0.9824020343219322</v>
+        <v>0.9924785550969049</v>
       </c>
     </row>
     <row r="193">
       <c r="A193">
-        <v>0.01202770432201133</v>
+        <v>0.005032455076956128</v>
       </c>
       <c r="B193">
         <v>20</v>
@@ -4413,12 +4413,12 @@
         </is>
       </c>
       <c r="E193">
-        <v>0.9944297386439436</v>
+        <v>0.997511010173861</v>
       </c>
     </row>
     <row r="194">
       <c r="A194">
-        <v>0.00259958712439789</v>
+        <v>0.001601270581736155</v>
       </c>
       <c r="B194">
         <v>21</v>
@@ -4434,12 +4434,12 @@
         </is>
       </c>
       <c r="E194">
-        <v>0.9970293257683415</v>
+        <v>0.9991122807555971</v>
       </c>
     </row>
     <row r="195">
       <c r="A195">
-        <v>0.001860049407974352</v>
+        <v>0.0006176438995196956</v>
       </c>
       <c r="B195">
         <v>22</v>
@@ -4455,12 +4455,12 @@
         </is>
       </c>
       <c r="E195">
-        <v>0.9988893751763158</v>
+        <v>0.9997299246551168</v>
       </c>
     </row>
     <row r="196">
       <c r="A196">
-        <v>0.0003374717565141277</v>
+        <v>0.0001189252228888855</v>
       </c>
       <c r="B196">
         <v>23</v>
@@ -4476,7 +4476,7 @@
         </is>
       </c>
       <c r="E196">
-        <v>0.9992268469328299</v>
+        <v>0.9998488498780057</v>
       </c>
     </row>
     <row r="197">
@@ -4497,12 +4497,12 @@
         </is>
       </c>
       <c r="E197">
-        <v>0.9992268469328299</v>
+        <v>0.9998488498780057</v>
       </c>
     </row>
     <row r="198">
       <c r="A198">
-        <v>1.977373573324967e-06</v>
+        <v>7.672595025089386e-07</v>
       </c>
       <c r="B198">
         <v>25</v>
@@ -4518,12 +4518,12 @@
         </is>
       </c>
       <c r="E198">
-        <v>0.9992288243064033</v>
+        <v>0.9998496171375082</v>
       </c>
     </row>
     <row r="199">
       <c r="A199">
-        <v>0.000771175693596737</v>
+        <v>0.000150382862491752</v>
       </c>
       <c r="B199">
         <v>26</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="205">
       <c r="A205">
-        <v>0.004812716572245751</v>
+        <v>0.1464396284829721</v>
       </c>
       <c r="B205">
         <v>6</v>
@@ -4665,12 +4665,12 @@
         </is>
       </c>
       <c r="E205">
-        <v>0.004812716572245751</v>
+        <v>0.1464396284829721</v>
       </c>
     </row>
     <row r="206">
       <c r="A206">
-        <v>0.003877674495352291</v>
+        <v>0.00913312693498452</v>
       </c>
       <c r="B206">
         <v>7</v>
@@ -4686,12 +4686,12 @@
         </is>
       </c>
       <c r="E206">
-        <v>0.00869039106759804</v>
+        <v>0.1555727554179566</v>
       </c>
     </row>
     <row r="207">
       <c r="A207">
-        <v>0.004290193058687641</v>
+        <v>0.006191950464396285</v>
       </c>
       <c r="B207">
         <v>8</v>
@@ -4707,12 +4707,12 @@
         </is>
       </c>
       <c r="E207">
-        <v>0.01298058412628568</v>
+        <v>0.1617647058823529</v>
       </c>
     </row>
     <row r="208">
       <c r="A208">
-        <v>0.005582751223805071</v>
+        <v>0.005030959752321981</v>
       </c>
       <c r="B208">
         <v>9</v>
@@ -4728,12 +4728,12 @@
         </is>
       </c>
       <c r="E208">
-        <v>0.01856333535009076</v>
+        <v>0.1667956656346749</v>
       </c>
     </row>
     <row r="209">
       <c r="A209">
-        <v>0.009982949232715472</v>
+        <v>0.0206656346749226</v>
       </c>
       <c r="B209">
         <v>10</v>
@@ -4749,12 +4749,12 @@
         </is>
       </c>
       <c r="E209">
-        <v>0.02854628458280623</v>
+        <v>0.1874613003095975</v>
       </c>
     </row>
     <row r="210">
       <c r="A210">
-        <v>0.01732577966008471</v>
+        <v>0.04109907120743034</v>
       </c>
       <c r="B210">
         <v>11</v>
@@ -4770,12 +4770,12 @@
         </is>
       </c>
       <c r="E210">
-        <v>0.04587206424289093</v>
+        <v>0.2285603715170278</v>
       </c>
     </row>
     <row r="211">
       <c r="A211">
-        <v>0.01091799130960893</v>
+        <v>0.03010835913312693</v>
       </c>
       <c r="B211">
         <v>12</v>
@@ -4791,12 +4791,12 @@
         </is>
       </c>
       <c r="E211">
-        <v>0.05679005555249986</v>
+        <v>0.2586687306501548</v>
       </c>
     </row>
     <row r="212">
       <c r="A212">
-        <v>0.005912766074473351</v>
+        <v>0.008978328173374612</v>
       </c>
       <c r="B212">
         <v>13</v>
@@ -4812,12 +4812,12 @@
         </is>
       </c>
       <c r="E212">
-        <v>0.06270282162697322</v>
+        <v>0.2676470588235294</v>
       </c>
     </row>
     <row r="213">
       <c r="A213">
-        <v>0.004785215334690061</v>
+        <v>0.00239938080495356</v>
       </c>
       <c r="B213">
         <v>14</v>
@@ -4833,12 +4833,12 @@
         </is>
       </c>
       <c r="E213">
-        <v>0.06748803696166328</v>
+        <v>0.270046439628483</v>
       </c>
     </row>
     <row r="214">
       <c r="A214">
-        <v>0.002502612617567791</v>
+        <v>0.164938080495356</v>
       </c>
       <c r="B214">
         <v>15</v>
@@ -4854,12 +4854,12 @@
         </is>
       </c>
       <c r="E214">
-        <v>0.06999064957923107</v>
+        <v>0.434984520123839</v>
       </c>
     </row>
     <row r="215">
       <c r="A215">
-        <v>0.27022716022221</v>
+        <v>0.1519349845201238</v>
       </c>
       <c r="B215">
         <v>16</v>
@@ -4875,12 +4875,12 @@
         </is>
       </c>
       <c r="E215">
-        <v>0.3402178098014411</v>
+        <v>0.5869195046439628</v>
       </c>
     </row>
     <row r="216">
       <c r="A216">
-        <v>0.2720147406633299</v>
+        <v>0.1419504643962848</v>
       </c>
       <c r="B216">
         <v>17</v>
@@ -4896,12 +4896,12 @@
         </is>
       </c>
       <c r="E216">
-        <v>0.6122325504647709</v>
+        <v>0.7288699690402477</v>
       </c>
     </row>
     <row r="217">
       <c r="A217">
-        <v>0.1402013090589077</v>
+        <v>0.1077399380804954</v>
       </c>
       <c r="B217">
         <v>18</v>
@@ -4917,12 +4917,12 @@
         </is>
       </c>
       <c r="E217">
-        <v>0.7524338595236786</v>
+        <v>0.836609907120743</v>
       </c>
     </row>
     <row r="218">
       <c r="A218">
-        <v>0.1410813486606897</v>
+        <v>0.09295665634674923</v>
       </c>
       <c r="B218">
         <v>19</v>
@@ -4938,12 +4938,12 @@
         </is>
       </c>
       <c r="E218">
-        <v>0.8935152081843682</v>
+        <v>0.9295665634674922</v>
       </c>
     </row>
     <row r="219">
       <c r="A219">
-        <v>0.07279577580991145</v>
+        <v>0.04713622291021672</v>
       </c>
       <c r="B219">
         <v>20</v>
@@ -4959,12 +4959,12 @@
         </is>
       </c>
       <c r="E219">
-        <v>0.9663109839942797</v>
+        <v>0.976702786377709</v>
       </c>
     </row>
     <row r="220">
       <c r="A220">
-        <v>0.01573070788185468</v>
+        <v>0.01501547987616099</v>
       </c>
       <c r="B220">
         <v>21</v>
@@ -4980,12 +4980,12 @@
         </is>
       </c>
       <c r="E220">
-        <v>0.9820416918761344</v>
+        <v>0.9917182662538699</v>
       </c>
     </row>
     <row r="221">
       <c r="A221">
-        <v>0.01124800616027721</v>
+        <v>0.005804953560371517</v>
       </c>
       <c r="B221">
         <v>22</v>
@@ -5001,12 +5001,12 @@
         </is>
       </c>
       <c r="E221">
-        <v>0.9932896980364117</v>
+        <v>0.9975232198142415</v>
       </c>
     </row>
     <row r="222">
       <c r="A222">
-        <v>0.00203509157912106</v>
+        <v>0.00108359133126935</v>
       </c>
       <c r="B222">
         <v>23</v>
@@ -5022,7 +5022,7 @@
         </is>
       </c>
       <c r="E222">
-        <v>0.9953247896155327</v>
+        <v>0.9986068111455109</v>
       </c>
     </row>
     <row r="223">
@@ -5043,7 +5043,7 @@
         </is>
       </c>
       <c r="E223">
-        <v>0.9953247896155327</v>
+        <v>0.9986068111455109</v>
       </c>
     </row>
     <row r="224">
@@ -5064,12 +5064,12 @@
         </is>
       </c>
       <c r="E224">
-        <v>0.9953247896155327</v>
+        <v>0.9986068111455109</v>
       </c>
     </row>
     <row r="225">
       <c r="A225">
-        <v>0.004675210384467301</v>
+        <v>0.001393188854489164</v>
       </c>
       <c r="B225">
         <v>26</v>

</xml_diff>